<commit_message>
Initial commit of Puralox app
</commit_message>
<xml_diff>
--- a/uploads/Purlox.xlsx
+++ b/uploads/Purlox.xlsx
@@ -1599,6 +1599,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1607,6 +1634,27 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1653,56 +1701,8 @@
     <xf numFmtId="21" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2151,11 +2151,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="226686464"/>
-        <c:axId val="226688384"/>
+        <c:axId val="233628800"/>
+        <c:axId val="233630720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="226686464"/>
+        <c:axId val="233628800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2203,13 +2203,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="226688384"/>
+        <c:crossAx val="233630720"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="226688384"/>
+        <c:axId val="233630720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="360"/>
@@ -2240,7 +2240,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="226686464"/>
+        <c:crossAx val="233628800"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="120"/>
@@ -2319,7 +2319,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2519,11 +2518,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="227098624"/>
-        <c:axId val="227100544"/>
+        <c:axId val="234032512"/>
+        <c:axId val="234038784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="227098624"/>
+        <c:axId val="234032512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -2548,7 +2547,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2572,13 +2570,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="227100544"/>
+        <c:crossAx val="234038784"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.05"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="227100544"/>
+        <c:axId val="234038784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.8000000000000002E-2"/>
@@ -2603,14 +2601,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="227098624"/>
+        <c:crossAx val="234032512"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="6.000000000000001E-3"/>
@@ -2828,11 +2825,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="226906496"/>
-        <c:axId val="226908416"/>
+        <c:axId val="233848832"/>
+        <c:axId val="233850752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="226906496"/>
+        <c:axId val="233848832"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2881,12 +2878,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="226908416"/>
+        <c:crossAx val="233850752"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="226908416"/>
+        <c:axId val="233850752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.60000000000000009"/>
@@ -2917,7 +2914,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="226906496"/>
+        <c:crossAx val="233848832"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.20000000000000004"/>
@@ -2989,7 +2986,7 @@
         <xdr:cNvPr id="2049" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E5858102-EC2F-41C4-8FD3-3C059459345E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5858102-EC2F-41C4-8FD3-3C059459345E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3205,7 +3202,7 @@
         <xdr:cNvPr id="3073" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AB6899C5-DD47-4E9A-922C-5E22F2ADEE98}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB6899C5-DD47-4E9A-922C-5E22F2ADEE98}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3445,7 +3442,7 @@
         <xdr:cNvPr id="4097" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EDDE8A95-8EE1-427C-B00B-992A77B29C52}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDDE8A95-8EE1-427C-B00B-992A77B29C52}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3906,7 +3903,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3941,151 +3938,151 @@
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="42" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="44"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="60"/>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="39">
+      <c r="B3" s="39"/>
+      <c r="C3" s="55">
         <v>44536</v>
       </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="41"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="57"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="51">
+      <c r="B4" s="39"/>
+      <c r="C4" s="67">
         <v>0.60168981481481476</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="47"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="63"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="45" t="s">
+      <c r="B5" s="39"/>
+      <c r="C5" s="61" t="s">
         <v>109</v>
       </c>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="47"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="63"/>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="45" t="s">
+      <c r="B6" s="39"/>
+      <c r="C6" s="61" t="s">
         <v>110</v>
       </c>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="47"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="63"/>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="45" t="s">
+      <c r="B7" s="39"/>
+      <c r="C7" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="47"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="63"/>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="B8" s="60"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="47"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="63"/>
     </row>
     <row r="9" spans="1:9" ht="15" customHeight="1">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="60"/>
-      <c r="C9" s="45">
+      <c r="B9" s="39"/>
+      <c r="C9" s="61">
         <v>494</v>
       </c>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="47"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="63"/>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1">
-      <c r="A10" s="67" t="s">
+      <c r="A10" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="B10" s="68"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="50"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="66"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1">
-      <c r="A12" s="52" t="s">
+      <c r="A12" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="62"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="6">
         <v>0.1812</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F12" s="52" t="s">
+      <c r="F12" s="42" t="s">
         <v>83</v>
       </c>
-      <c r="G12" s="53"/>
+      <c r="G12" s="68"/>
       <c r="H12" s="8">
         <v>101.33</v>
       </c>
@@ -4094,20 +4091,20 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1">
-      <c r="A13" s="54" t="s">
+      <c r="A13" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="B13" s="56"/>
+      <c r="B13" s="41"/>
       <c r="C13" s="9">
         <v>9.0739999999999998</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="F13" s="54" t="s">
+      <c r="F13" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="G13" s="55"/>
+      <c r="G13" s="47"/>
       <c r="H13" s="11">
         <v>0.16200000000000001</v>
       </c>
@@ -4116,106 +4113,106 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="B14" s="56"/>
+      <c r="B14" s="41"/>
       <c r="C14" s="9">
         <v>15.766</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="F14" s="54" t="s">
+      <c r="F14" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="G14" s="55"/>
+      <c r="G14" s="47"/>
       <c r="H14" s="4"/>
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" ht="15" customHeight="1">
-      <c r="A15" s="54" t="s">
+      <c r="A15" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="B15" s="56"/>
+      <c r="B15" s="41"/>
       <c r="C15" s="9">
         <v>0</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="F15" s="54" t="s">
+      <c r="F15" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="G15" s="55"/>
+      <c r="G15" s="47"/>
       <c r="H15" s="4"/>
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" ht="15" customHeight="1">
-      <c r="A16" s="54" t="s">
+      <c r="A16" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="B16" s="56"/>
+      <c r="B16" s="41"/>
       <c r="C16" s="9" t="s">
         <v>112</v>
       </c>
       <c r="D16" s="10"/>
-      <c r="F16" s="54" t="s">
+      <c r="F16" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="G16" s="55"/>
+      <c r="G16" s="47"/>
       <c r="H16" s="4"/>
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" ht="15" customHeight="1">
-      <c r="A17" s="54" t="s">
+      <c r="A17" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="B17" s="56"/>
+      <c r="B17" s="41"/>
       <c r="C17" s="9">
         <v>0</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="F17" s="54" t="s">
+      <c r="F17" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="G17" s="55"/>
+      <c r="G17" s="47"/>
       <c r="H17" s="4">
         <v>30</v>
       </c>
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" ht="15" customHeight="1">
-      <c r="A18" s="65" t="s">
+      <c r="A18" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="B18" s="64"/>
+      <c r="B18" s="37"/>
       <c r="C18" s="12">
         <v>77</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F18" s="65" t="s">
+      <c r="F18" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="G18" s="66"/>
+      <c r="G18" s="48"/>
       <c r="H18" s="5">
         <v>20</v>
       </c>
       <c r="I18" s="13"/>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="B20" s="35"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="36"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="45"/>
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1">
       <c r="A21" s="15" t="s">
@@ -4286,24 +4283,24 @@
       <c r="F25" s="13"/>
     </row>
     <row r="26" spans="1:9" ht="15" customHeight="1">
-      <c r="A26" s="34" t="s">
+      <c r="A26" s="43" t="s">
         <v>107</v>
       </c>
-      <c r="B26" s="35"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="36"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="45"/>
     </row>
     <row r="27" spans="1:9" ht="15" customHeight="1">
       <c r="A27" s="17" t="s">
         <v>105</v>
       </c>
       <c r="B27" s="18"/>
-      <c r="C27" s="37" t="s">
+      <c r="C27" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="D27" s="38"/>
+      <c r="D27" s="54"/>
       <c r="E27" s="17"/>
       <c r="F27" s="18"/>
     </row>
@@ -4312,10 +4309,10 @@
         <v>106</v>
       </c>
       <c r="B28" s="7"/>
-      <c r="C28" s="61">
+      <c r="C28" s="34">
         <v>0.41399999999999998</v>
       </c>
-      <c r="D28" s="62"/>
+      <c r="D28" s="35"/>
       <c r="E28" s="14" t="s">
         <v>125</v>
       </c>
@@ -4326,10 +4323,10 @@
         <v>128</v>
       </c>
       <c r="B29" s="13"/>
-      <c r="C29" s="63">
+      <c r="C29" s="36">
         <v>145.09</v>
       </c>
-      <c r="D29" s="64"/>
+      <c r="D29" s="37"/>
       <c r="E29" s="16" t="s">
         <v>123</v>
       </c>
@@ -4337,6 +4334,27 @@
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="C2:I2"/>
+    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="C10:I10"/>
+    <mergeCell ref="C8:I8"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="A6:B6"/>
@@ -4353,27 +4371,6 @@
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A26:F26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="C2:I2"/>
-    <mergeCell ref="C9:I9"/>
-    <mergeCell ref="C10:I10"/>
-    <mergeCell ref="C8:I8"/>
-    <mergeCell ref="C7:I7"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="A16:B16"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51200000000000001" footer="0.51200000000000001"/>
@@ -4402,151 +4399,151 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="42" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="44"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="60"/>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="39">
+      <c r="B3" s="39"/>
+      <c r="C3" s="55">
         <v>44536</v>
       </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="41"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="57"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="51">
+      <c r="B4" s="39"/>
+      <c r="C4" s="67">
         <v>0.60168981481481476</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="47"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="63"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="45" t="s">
+      <c r="B5" s="39"/>
+      <c r="C5" s="61" t="s">
         <v>109</v>
       </c>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="47"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="63"/>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="45" t="s">
+      <c r="B6" s="39"/>
+      <c r="C6" s="61" t="s">
         <v>110</v>
       </c>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="47"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="63"/>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="45" t="s">
+      <c r="B7" s="39"/>
+      <c r="C7" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="47"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="63"/>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="60"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="47"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="63"/>
     </row>
     <row r="9" spans="1:9" ht="15" customHeight="1">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="60"/>
-      <c r="C9" s="45">
+      <c r="B9" s="39"/>
+      <c r="C9" s="61">
         <v>494</v>
       </c>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="47"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="63"/>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1">
-      <c r="A10" s="67" t="s">
+      <c r="A10" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="68"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="50"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="66"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1">
-      <c r="A12" s="52" t="s">
+      <c r="A12" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="62"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="6">
         <v>0.1812</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F12" s="52" t="s">
+      <c r="F12" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="53"/>
+      <c r="G12" s="68"/>
       <c r="H12" s="8">
         <v>101.33</v>
       </c>
@@ -4555,20 +4552,20 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1">
-      <c r="A13" s="54" t="s">
+      <c r="A13" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="56"/>
+      <c r="B13" s="41"/>
       <c r="C13" s="9">
         <v>9.0739999999999998</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="54" t="s">
+      <c r="F13" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="55"/>
+      <c r="G13" s="47"/>
       <c r="H13" s="11">
         <v>0.16200000000000001</v>
       </c>
@@ -4577,92 +4574,92 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="56"/>
+      <c r="B14" s="41"/>
       <c r="C14" s="9">
         <v>15.766</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="54" t="s">
+      <c r="F14" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="55"/>
+      <c r="G14" s="47"/>
       <c r="H14" s="4"/>
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" ht="15" customHeight="1">
-      <c r="A15" s="54" t="s">
+      <c r="A15" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="56"/>
+      <c r="B15" s="41"/>
       <c r="C15" s="9">
         <v>0</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="F15" s="54" t="s">
+      <c r="F15" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="55"/>
+      <c r="G15" s="47"/>
       <c r="H15" s="4"/>
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" ht="15" customHeight="1">
-      <c r="A16" s="54" t="s">
+      <c r="A16" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="56"/>
+      <c r="B16" s="41"/>
       <c r="C16" s="9" t="s">
         <v>112</v>
       </c>
       <c r="D16" s="10"/>
-      <c r="F16" s="54" t="s">
+      <c r="F16" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="G16" s="55"/>
+      <c r="G16" s="47"/>
       <c r="H16" s="4"/>
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" ht="15" customHeight="1">
-      <c r="A17" s="54" t="s">
+      <c r="A17" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="56"/>
+      <c r="B17" s="41"/>
       <c r="C17" s="9">
         <v>0</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="54" t="s">
+      <c r="F17" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="55"/>
+      <c r="G17" s="47"/>
       <c r="H17" s="4">
         <v>30</v>
       </c>
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" ht="15" customHeight="1">
-      <c r="A18" s="65" t="s">
+      <c r="A18" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="64"/>
+      <c r="B18" s="37"/>
       <c r="C18" s="12">
         <v>77</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F18" s="65" t="s">
+      <c r="F18" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="66"/>
+      <c r="G18" s="48"/>
       <c r="H18" s="5">
         <v>20</v>
       </c>
@@ -5874,14 +5871,15 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C2:I2"/>
+    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="C10:I10"/>
+    <mergeCell ref="C8:I8"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="C3:I3"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="F17:G17"/>
@@ -5897,15 +5895,14 @@
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C2:I2"/>
-    <mergeCell ref="C9:I9"/>
-    <mergeCell ref="C10:I10"/>
-    <mergeCell ref="C8:I8"/>
-    <mergeCell ref="C7:I7"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51200000000000001" footer="0.51200000000000001"/>
@@ -5937,19 +5934,19 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="42" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="44"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="60"/>
       <c r="O2" s="3">
         <v>0</v>
       </c>
@@ -5958,19 +5955,19 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="39">
+      <c r="B3" s="39"/>
+      <c r="C3" s="55">
         <v>44536</v>
       </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="41"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="57"/>
       <c r="O3" s="3">
         <v>0.5</v>
       </c>
@@ -5979,123 +5976,123 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="51">
+      <c r="B4" s="39"/>
+      <c r="C4" s="67">
         <v>0.60168981481481476</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="47"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="63"/>
     </row>
     <row r="5" spans="1:16" ht="15" customHeight="1">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="45" t="s">
+      <c r="B5" s="39"/>
+      <c r="C5" s="61" t="s">
         <v>109</v>
       </c>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="47"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="63"/>
     </row>
     <row r="6" spans="1:16" ht="15" customHeight="1">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="45" t="s">
+      <c r="B6" s="39"/>
+      <c r="C6" s="61" t="s">
         <v>110</v>
       </c>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="47"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="63"/>
     </row>
     <row r="7" spans="1:16" ht="15" customHeight="1">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="45" t="s">
+      <c r="B7" s="39"/>
+      <c r="C7" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="47"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="63"/>
     </row>
     <row r="8" spans="1:16" ht="15" customHeight="1">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="60"/>
-      <c r="C8" s="45" t="s">
+      <c r="B8" s="39"/>
+      <c r="C8" s="61" t="s">
         <v>132</v>
       </c>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="47"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="63"/>
     </row>
     <row r="9" spans="1:16" ht="15" customHeight="1">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="60"/>
-      <c r="C9" s="45">
+      <c r="B9" s="39"/>
+      <c r="C9" s="61">
         <v>494</v>
       </c>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="47"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="63"/>
     </row>
     <row r="10" spans="1:16" ht="15" customHeight="1">
-      <c r="A10" s="67" t="s">
+      <c r="A10" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="68"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="50"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="66"/>
     </row>
     <row r="12" spans="1:16" ht="15" customHeight="1">
-      <c r="A12" s="52" t="s">
+      <c r="A12" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="62"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="6">
         <v>0.1812</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F12" s="52" t="s">
+      <c r="F12" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="53"/>
+      <c r="G12" s="68"/>
       <c r="H12" s="8">
         <v>101.33</v>
       </c>
@@ -6104,20 +6101,20 @@
       </c>
     </row>
     <row r="13" spans="1:16" ht="15" customHeight="1">
-      <c r="A13" s="54" t="s">
+      <c r="A13" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="56"/>
+      <c r="B13" s="41"/>
       <c r="C13" s="9">
         <v>9.0739999999999998</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="F13" s="54" t="s">
+      <c r="F13" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="G13" s="55"/>
+      <c r="G13" s="47"/>
       <c r="H13" s="11">
         <v>0.16200000000000001</v>
       </c>
@@ -6126,92 +6123,92 @@
       </c>
     </row>
     <row r="14" spans="1:16" ht="15" customHeight="1">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="56"/>
+      <c r="B14" s="41"/>
       <c r="C14" s="9">
         <v>15.766</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="54" t="s">
+      <c r="F14" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="G14" s="55"/>
+      <c r="G14" s="47"/>
       <c r="H14" s="4"/>
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:16" ht="15" customHeight="1">
-      <c r="A15" s="54" t="s">
+      <c r="A15" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="56"/>
+      <c r="B15" s="41"/>
       <c r="C15" s="9">
         <v>0</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="54" t="s">
+      <c r="F15" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="55"/>
+      <c r="G15" s="47"/>
       <c r="H15" s="4"/>
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:16" ht="15" customHeight="1">
-      <c r="A16" s="54" t="s">
+      <c r="A16" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="56"/>
+      <c r="B16" s="41"/>
       <c r="C16" s="9" t="s">
         <v>112</v>
       </c>
       <c r="D16" s="10"/>
-      <c r="F16" s="54" t="s">
+      <c r="F16" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="G16" s="55"/>
+      <c r="G16" s="47"/>
       <c r="H16" s="4"/>
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" ht="15" customHeight="1">
-      <c r="A17" s="54" t="s">
+      <c r="A17" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="56"/>
+      <c r="B17" s="41"/>
       <c r="C17" s="9">
         <v>0</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F17" s="54" t="s">
+      <c r="F17" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="55"/>
+      <c r="G17" s="47"/>
       <c r="H17" s="4">
         <v>30</v>
       </c>
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" ht="15" customHeight="1">
-      <c r="A18" s="65" t="s">
+      <c r="A18" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="64"/>
+      <c r="B18" s="37"/>
       <c r="C18" s="12">
         <v>77</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F18" s="65" t="s">
+      <c r="F18" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="66"/>
+      <c r="G18" s="48"/>
       <c r="H18" s="5">
         <v>20</v>
       </c>
@@ -6539,11 +6536,25 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
     <mergeCell ref="C2:I2"/>
     <mergeCell ref="C9:I9"/>
     <mergeCell ref="C10:I10"/>
@@ -6552,25 +6563,11 @@
     <mergeCell ref="C6:I6"/>
     <mergeCell ref="C5:I5"/>
     <mergeCell ref="C4:I4"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="C3:I3"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51200000000000001" footer="0.51200000000000001"/>
@@ -6602,153 +6599,153 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="42" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="44"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="60"/>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="39">
+      <c r="B3" s="39"/>
+      <c r="C3" s="55">
         <v>44536</v>
       </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="41"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="57"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="51">
+      <c r="B4" s="39"/>
+      <c r="C4" s="67">
         <v>0.60168981481481476</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="46"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="47"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="63"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="45" t="s">
+      <c r="B5" s="39"/>
+      <c r="C5" s="61" t="s">
         <v>109</v>
       </c>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="47"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="63"/>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="45" t="s">
+      <c r="B6" s="39"/>
+      <c r="C6" s="61" t="s">
         <v>110</v>
       </c>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="47"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="63"/>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="45" t="s">
+      <c r="B7" s="39"/>
+      <c r="C7" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="47"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="63"/>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="60"/>
-      <c r="C8" s="45" t="s">
+      <c r="B8" s="39"/>
+      <c r="C8" s="61" t="s">
         <v>132</v>
       </c>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="47"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="63"/>
     </row>
     <row r="9" spans="1:9" ht="15" customHeight="1">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="60"/>
-      <c r="C9" s="45">
+      <c r="B9" s="39"/>
+      <c r="C9" s="61">
         <v>494</v>
       </c>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="47"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="63"/>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1">
-      <c r="A10" s="67" t="s">
+      <c r="A10" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="68"/>
-      <c r="C10" s="48"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="50"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="66"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1">
-      <c r="A12" s="52" t="s">
+      <c r="A12" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="62"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="6">
         <v>0.1812</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F12" s="52" t="s">
+      <c r="F12" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="53"/>
+      <c r="G12" s="68"/>
       <c r="H12" s="8">
         <v>101.33</v>
       </c>
@@ -6757,20 +6754,20 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1">
-      <c r="A13" s="54" t="s">
+      <c r="A13" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="56"/>
+      <c r="B13" s="41"/>
       <c r="C13" s="9">
         <v>9.0739999999999998</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="F13" s="54" t="s">
+      <c r="F13" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="G13" s="55"/>
+      <c r="G13" s="47"/>
       <c r="H13" s="11">
         <v>0.16200000000000001</v>
       </c>
@@ -6779,92 +6776,92 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="56"/>
+      <c r="B14" s="41"/>
       <c r="C14" s="9">
         <v>15.766</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="54" t="s">
+      <c r="F14" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="G14" s="55"/>
+      <c r="G14" s="47"/>
       <c r="H14" s="4"/>
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" ht="15" customHeight="1">
-      <c r="A15" s="54" t="s">
+      <c r="A15" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="56"/>
+      <c r="B15" s="41"/>
       <c r="C15" s="9">
         <v>0</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="54" t="s">
+      <c r="F15" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="55"/>
+      <c r="G15" s="47"/>
       <c r="H15" s="4"/>
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" ht="15" customHeight="1">
-      <c r="A16" s="54" t="s">
+      <c r="A16" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="56"/>
+      <c r="B16" s="41"/>
       <c r="C16" s="9" t="s">
         <v>112</v>
       </c>
       <c r="D16" s="10"/>
-      <c r="F16" s="54" t="s">
+      <c r="F16" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="G16" s="55"/>
+      <c r="G16" s="47"/>
       <c r="H16" s="4"/>
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" ht="15" customHeight="1">
-      <c r="A17" s="54" t="s">
+      <c r="A17" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="56"/>
+      <c r="B17" s="41"/>
       <c r="C17" s="9">
         <v>0</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F17" s="54" t="s">
+      <c r="F17" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="55"/>
+      <c r="G17" s="47"/>
       <c r="H17" s="4">
         <v>30</v>
       </c>
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" ht="15" customHeight="1">
-      <c r="A18" s="65" t="s">
+      <c r="A18" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="64"/>
+      <c r="B18" s="37"/>
       <c r="C18" s="12">
         <v>77</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F18" s="65" t="s">
+      <c r="F18" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="66"/>
+      <c r="G18" s="48"/>
       <c r="H18" s="5">
         <v>20</v>
       </c>
@@ -6875,7 +6872,7 @@
         <v>47</v>
       </c>
       <c r="B20" s="18"/>
-      <c r="C20" s="37" t="s">
+      <c r="C20" s="53" t="s">
         <v>127</v>
       </c>
       <c r="D20" s="69"/>
@@ -6886,7 +6883,7 @@
         <v>46</v>
       </c>
       <c r="B21" s="7"/>
-      <c r="C21" s="61">
+      <c r="C21" s="34">
         <v>0.41399999999999998</v>
       </c>
       <c r="D21" s="70"/>
@@ -6899,7 +6896,7 @@
         <v>128</v>
       </c>
       <c r="B22" s="13"/>
-      <c r="C22" s="63">
+      <c r="C22" s="36">
         <v>145.09</v>
       </c>
       <c r="D22" s="71"/>
@@ -7205,13 +7202,25 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
     <mergeCell ref="C3:I3"/>
     <mergeCell ref="C2:I2"/>
     <mergeCell ref="C9:I9"/>
@@ -7221,25 +7230,13 @@
     <mergeCell ref="C6:I6"/>
     <mergeCell ref="C5:I5"/>
     <mergeCell ref="C4:I4"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F14:G14"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51200000000000001" footer="0.51200000000000001"/>

</xml_diff>